<commit_message>
Generate Java code from only declared columns of an Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/yokohama/unit/translator/TestExcel.xlsx
+++ b/src/test/resources/yokohama/unit/translator/TestExcel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>sut</t>
   </si>
@@ -46,6 +46,22 @@
   </si>
   <si>
     <t>false</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>dummy</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>""</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -707,12 +723,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="C3:E6" totalsRowShown="0">
-  <autoFilter ref="C3:E6"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="C3:F6" totalsRowShown="0">
+  <autoFilter ref="C3:F6"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="sut"/>
     <tableColumn id="2" name="prefix"/>
     <tableColumn id="3" name="expected" dataDxfId="0"/>
+    <tableColumn id="4" name="dummy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1005,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E6"/>
+  <dimension ref="C3:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1018,7 +1035,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -1028,8 +1045,11 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -1039,8 +1059,11 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -1050,8 +1073,11 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -1060,6 +1086,9 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>